<commit_message>
최종빌드 alpha ver 0.5 /
</commit_message>
<xml_diff>
--- a/05.일정관리/WBS template.xlsx
+++ b/05.일정관리/WBS template.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="125">
   <si>
     <t>공정</t>
   </si>
@@ -477,6 +477,18 @@
   </si>
   <si>
     <t>이경호</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ITCH.io 런칭</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>엔딩크레딧</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>전세현</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -708,23 +720,8 @@
     <xf numFmtId="176" fontId="4" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -740,6 +737,21 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -777,7 +789,7 @@
     <xdr:to>
       <xdr:col>18</xdr:col>
       <xdr:colOff>381001</xdr:colOff>
-      <xdr:row>58</xdr:row>
+      <xdr:row>60</xdr:row>
       <xdr:rowOff>149039</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -785,7 +797,7 @@
         <xdr:cNvPr id="2" name="직사각형 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -842,7 +854,7 @@
     <xdr:to>
       <xdr:col>20</xdr:col>
       <xdr:colOff>382682</xdr:colOff>
-      <xdr:row>58</xdr:row>
+      <xdr:row>60</xdr:row>
       <xdr:rowOff>156882</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -850,7 +862,7 @@
         <xdr:cNvPr id="3" name="직사각형 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -909,7 +921,7 @@
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>371475</xdr:colOff>
-      <xdr:row>58</xdr:row>
+      <xdr:row>60</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -917,7 +929,7 @@
         <xdr:cNvPr id="4" name="직사각형 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FB86EDE9-89EE-4017-A973-816CDCF02D0F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{FB86EDE9-89EE-4017-A973-816CDCF02D0F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1230,13 +1242,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AL66"/>
+  <dimension ref="A1:AL68"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="8" ySplit="4" topLeftCell="I11" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="8" ySplit="4" topLeftCell="I14" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="B40" sqref="B40"/>
+      <selection pane="bottomRight" activeCell="Y46" sqref="Y46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.125" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1248,45 +1260,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:38" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
-      <c r="M1" s="20"/>
-      <c r="N1" s="20"/>
-      <c r="O1" s="20"/>
-      <c r="P1" s="20"/>
-      <c r="Q1" s="20"/>
-      <c r="R1" s="20"/>
-      <c r="S1" s="20"/>
-      <c r="T1" s="20"/>
-      <c r="U1" s="20"/>
-      <c r="V1" s="20"/>
-      <c r="W1" s="20"/>
-      <c r="X1" s="20"/>
-      <c r="Y1" s="20"/>
-      <c r="Z1" s="20"/>
-      <c r="AA1" s="20"/>
-      <c r="AB1" s="20"/>
-      <c r="AC1" s="20"/>
-      <c r="AD1" s="20"/>
-      <c r="AE1" s="20"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="26"/>
+      <c r="P1" s="26"/>
+      <c r="Q1" s="26"/>
+      <c r="R1" s="26"/>
+      <c r="S1" s="26"/>
+      <c r="T1" s="26"/>
+      <c r="U1" s="26"/>
+      <c r="V1" s="26"/>
+      <c r="W1" s="26"/>
+      <c r="X1" s="26"/>
+      <c r="Y1" s="26"/>
+      <c r="Z1" s="26"/>
+      <c r="AA1" s="26"/>
+      <c r="AB1" s="26"/>
+      <c r="AC1" s="26"/>
+      <c r="AD1" s="26"/>
+      <c r="AE1" s="26"/>
     </row>
     <row r="2" spans="1:38" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="18" t="s">
         <v>120</v>
       </c>
       <c r="F2" s="2"/>
@@ -1316,28 +1328,28 @@
       <c r="AE2" s="1"/>
     </row>
     <row r="3" spans="1:38" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="D3" s="23" t="s">
+      <c r="D3" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="E3" s="23" t="s">
+      <c r="E3" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="F3" s="21" t="s">
+      <c r="F3" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="23" t="s">
+      <c r="G3" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="23" t="s">
+      <c r="H3" s="25" t="s">
         <v>39</v>
       </c>
       <c r="I3" s="4" t="s">
@@ -1432,14 +1444,14 @@
       </c>
     </row>
     <row r="4" spans="1:38" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="23"/>
-      <c r="B4" s="23"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="23"/>
+      <c r="A4" s="25"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="25"/>
       <c r="I4" s="4">
         <v>43864</v>
       </c>
@@ -1482,11 +1494,21 @@
       <c r="V4" s="15">
         <v>43877</v>
       </c>
-      <c r="W4" s="4"/>
-      <c r="X4" s="4"/>
-      <c r="Y4" s="4"/>
-      <c r="Z4" s="4"/>
-      <c r="AA4" s="4"/>
+      <c r="W4" s="4">
+        <v>43878</v>
+      </c>
+      <c r="X4" s="4">
+        <v>43879</v>
+      </c>
+      <c r="Y4" s="4">
+        <v>43880</v>
+      </c>
+      <c r="Z4" s="4">
+        <v>43881</v>
+      </c>
+      <c r="AA4" s="4">
+        <v>43882</v>
+      </c>
       <c r="AB4" s="4"/>
       <c r="AC4" s="4"/>
       <c r="AD4" s="4"/>
@@ -1503,11 +1525,11 @@
       <c r="A5" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="25" t="s">
+      <c r="B5" s="20" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="13" t="s">
@@ -1555,10 +1577,12 @@
     </row>
     <row r="6" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A6" s="24"/>
-      <c r="B6" s="25" t="s">
+      <c r="B6" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="8"/>
+      <c r="C6" s="14">
+        <v>1</v>
+      </c>
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
       <c r="F6" s="7">
@@ -1603,10 +1627,12 @@
     </row>
     <row r="7" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A7" s="24"/>
-      <c r="B7" s="25" t="s">
+      <c r="B7" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="C7" s="8"/>
+      <c r="C7" s="14">
+        <v>1</v>
+      </c>
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
       <c r="F7" s="7">
@@ -1654,7 +1680,9 @@
       <c r="B8" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="C8" s="8"/>
+      <c r="C8" s="14">
+        <v>0.95</v>
+      </c>
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
       <c r="F8" s="7">
@@ -1699,10 +1727,12 @@
     </row>
     <row r="9" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A9" s="24"/>
-      <c r="B9" s="25" t="s">
+      <c r="B9" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="C9" s="8"/>
+      <c r="C9" s="14">
+        <v>1</v>
+      </c>
       <c r="D9" s="8"/>
       <c r="E9" s="8"/>
       <c r="F9" s="7">
@@ -1747,10 +1777,12 @@
     </row>
     <row r="10" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A10" s="24"/>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="C10" s="8"/>
+      <c r="C10" s="14">
+        <v>1</v>
+      </c>
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
       <c r="F10" s="7">
@@ -1794,28 +1826,20 @@
       <c r="AL10" s="8"/>
     </row>
     <row r="11" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A11" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="B11" s="25" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="8"/>
+      <c r="A11" s="19"/>
+      <c r="B11" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="C11" s="14"/>
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>
-      <c r="F11" s="7">
-        <v>43866</v>
-      </c>
-      <c r="G11" s="7">
-        <v>43868</v>
-      </c>
-      <c r="H11" s="12" t="s">
-        <v>96</v>
-      </c>
-      <c r="I11" s="9"/>
-      <c r="J11" s="9"/>
-      <c r="K11" s="9"/>
-      <c r="L11" s="9"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
       <c r="M11" s="10"/>
       <c r="N11" s="10"/>
       <c r="O11" s="10"/>
@@ -1823,7 +1847,7 @@
       <c r="Q11" s="10"/>
       <c r="R11" s="10"/>
       <c r="S11" s="10"/>
-      <c r="T11" s="10"/>
+      <c r="T11" s="9"/>
       <c r="U11" s="10"/>
       <c r="V11" s="10"/>
       <c r="W11" s="10"/>
@@ -1844,15 +1868,19 @@
       <c r="AL11" s="8"/>
     </row>
     <row r="12" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A12" s="24"/>
-      <c r="B12" s="26" t="s">
-        <v>90</v>
-      </c>
-      <c r="C12" s="8"/>
+      <c r="A12" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="14">
+        <v>1</v>
+      </c>
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
       <c r="F12" s="7">
-        <v>43864</v>
+        <v>43866</v>
       </c>
       <c r="G12" s="7">
         <v>43868</v>
@@ -1861,9 +1889,9 @@
         <v>96</v>
       </c>
       <c r="I12" s="9"/>
-      <c r="J12" s="10"/>
-      <c r="K12" s="10"/>
-      <c r="L12" s="10"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="9"/>
       <c r="M12" s="10"/>
       <c r="N12" s="10"/>
       <c r="O12" s="10"/>
@@ -1893,24 +1921,26 @@
     </row>
     <row r="13" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A13" s="24"/>
-      <c r="B13" s="26" t="s">
-        <v>59</v>
-      </c>
-      <c r="C13" s="8"/>
+      <c r="B13" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="C13" s="14">
+        <v>1</v>
+      </c>
       <c r="D13" s="8"/>
       <c r="E13" s="8"/>
       <c r="F13" s="7">
         <v>43864</v>
       </c>
       <c r="G13" s="7">
-        <v>43866</v>
+        <v>43868</v>
       </c>
       <c r="H13" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="I13" s="10"/>
-      <c r="J13" s="9"/>
-      <c r="K13" s="9"/>
+        <v>96</v>
+      </c>
+      <c r="I13" s="9"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10"/>
       <c r="L13" s="10"/>
       <c r="M13" s="10"/>
       <c r="N13" s="10"/>
@@ -1941,25 +1971,27 @@
     </row>
     <row r="14" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A14" s="24"/>
-      <c r="B14" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" s="8"/>
+      <c r="B14" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="C14" s="14">
+        <v>1</v>
+      </c>
       <c r="D14" s="8"/>
       <c r="E14" s="8"/>
       <c r="F14" s="7">
+        <v>43864</v>
+      </c>
+      <c r="G14" s="7">
         <v>43866</v>
-      </c>
-      <c r="G14" s="7">
-        <v>43867</v>
       </c>
       <c r="H14" s="12" t="s">
         <v>95</v>
       </c>
       <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
+      <c r="J14" s="9"/>
       <c r="K14" s="9"/>
-      <c r="L14" s="9"/>
+      <c r="L14" s="10"/>
       <c r="M14" s="10"/>
       <c r="N14" s="10"/>
       <c r="O14" s="10"/>
@@ -1989,14 +2021,16 @@
     </row>
     <row r="15" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A15" s="24"/>
-      <c r="B15" s="26" t="s">
-        <v>60</v>
-      </c>
-      <c r="C15" s="8"/>
+      <c r="B15" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="14">
+        <v>1</v>
+      </c>
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
       <c r="F15" s="7">
-        <v>43865</v>
+        <v>43866</v>
       </c>
       <c r="G15" s="7">
         <v>43867</v>
@@ -2005,7 +2039,7 @@
         <v>95</v>
       </c>
       <c r="I15" s="10"/>
-      <c r="J15" s="9"/>
+      <c r="J15" s="10"/>
       <c r="K15" s="9"/>
       <c r="L15" s="9"/>
       <c r="M15" s="10"/>
@@ -2037,27 +2071,29 @@
     </row>
     <row r="16" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A16" s="24"/>
-      <c r="B16" s="25" t="s">
-        <v>87</v>
-      </c>
-      <c r="C16" s="8"/>
+      <c r="B16" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="C16" s="14">
+        <v>1</v>
+      </c>
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
       <c r="F16" s="7">
+        <v>43865</v>
+      </c>
+      <c r="G16" s="7">
         <v>43867</v>
       </c>
-      <c r="G16" s="7">
-        <v>43869</v>
-      </c>
       <c r="H16" s="12" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="I16" s="10"/>
-      <c r="J16" s="10"/>
-      <c r="K16" s="10"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
       <c r="L16" s="9"/>
-      <c r="M16" s="9"/>
-      <c r="N16" s="9"/>
+      <c r="M16" s="10"/>
+      <c r="N16" s="10"/>
       <c r="O16" s="10"/>
       <c r="P16" s="10"/>
       <c r="Q16" s="10"/>
@@ -2085,27 +2121,29 @@
     </row>
     <row r="17" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A17" s="24"/>
-      <c r="B17" s="26" t="s">
-        <v>8</v>
-      </c>
-      <c r="C17" s="8"/>
+      <c r="B17" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="C17" s="14">
+        <v>1</v>
+      </c>
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
       <c r="F17" s="7">
         <v>43867</v>
       </c>
       <c r="G17" s="7">
-        <v>43867</v>
+        <v>43869</v>
       </c>
       <c r="H17" s="12" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="I17" s="10"/>
       <c r="J17" s="10"/>
       <c r="K17" s="10"/>
       <c r="L17" s="9"/>
-      <c r="M17" s="10"/>
-      <c r="N17" s="10"/>
+      <c r="M17" s="9"/>
+      <c r="N17" s="9"/>
       <c r="O17" s="10"/>
       <c r="P17" s="10"/>
       <c r="Q17" s="10"/>
@@ -2133,26 +2171,28 @@
     </row>
     <row r="18" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A18" s="24"/>
-      <c r="B18" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="C18" s="8"/>
+      <c r="B18" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="14">
+        <v>1</v>
+      </c>
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
       <c r="F18" s="7">
-        <v>43868</v>
+        <v>43867</v>
       </c>
       <c r="G18" s="7">
-        <v>43868</v>
+        <v>43867</v>
       </c>
       <c r="H18" s="12" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="I18" s="10"/>
       <c r="J18" s="10"/>
       <c r="K18" s="10"/>
-      <c r="L18" s="10"/>
-      <c r="M18" s="9"/>
+      <c r="L18" s="9"/>
+      <c r="M18" s="10"/>
       <c r="N18" s="10"/>
       <c r="O18" s="10"/>
       <c r="P18" s="10"/>
@@ -2181,26 +2221,28 @@
     </row>
     <row r="19" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A19" s="24"/>
-      <c r="B19" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="C19" s="8"/>
+      <c r="B19" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="C19" s="14">
+        <v>1</v>
+      </c>
       <c r="D19" s="8"/>
       <c r="E19" s="8"/>
       <c r="F19" s="7">
-        <v>43867</v>
+        <v>43868</v>
       </c>
       <c r="G19" s="7">
-        <v>43867</v>
+        <v>43868</v>
       </c>
       <c r="H19" s="12" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="I19" s="10"/>
       <c r="J19" s="10"/>
       <c r="K19" s="10"/>
-      <c r="L19" s="9"/>
-      <c r="M19" s="10"/>
+      <c r="L19" s="10"/>
+      <c r="M19" s="9"/>
       <c r="N19" s="10"/>
       <c r="O19" s="10"/>
       <c r="P19" s="10"/>
@@ -2229,30 +2271,34 @@
     </row>
     <row r="20" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A20" s="24"/>
-      <c r="B20" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C20" s="8"/>
+      <c r="B20" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="14">
+        <v>1</v>
+      </c>
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
       <c r="F20" s="7">
-        <v>43865</v>
+        <v>43867</v>
       </c>
       <c r="G20" s="7">
-        <v>43865</v>
-      </c>
-      <c r="H20" s="12"/>
+        <v>43867</v>
+      </c>
+      <c r="H20" s="12" t="s">
+        <v>89</v>
+      </c>
       <c r="I20" s="10"/>
-      <c r="J20" s="9"/>
-      <c r="K20" s="9"/>
+      <c r="J20" s="10"/>
+      <c r="K20" s="10"/>
       <c r="L20" s="9"/>
-      <c r="M20" s="9"/>
+      <c r="M20" s="10"/>
       <c r="N20" s="10"/>
       <c r="O20" s="10"/>
-      <c r="P20" s="9"/>
-      <c r="Q20" s="9"/>
-      <c r="R20" s="9"/>
-      <c r="S20" s="9"/>
+      <c r="P20" s="10"/>
+      <c r="Q20" s="10"/>
+      <c r="R20" s="10"/>
+      <c r="S20" s="10"/>
       <c r="T20" s="10"/>
       <c r="U20" s="10"/>
       <c r="V20" s="10"/>
@@ -2275,21 +2321,19 @@
     </row>
     <row r="21" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A21" s="24"/>
-      <c r="B21" s="26" t="s">
-        <v>61</v>
-      </c>
-      <c r="C21" s="8"/>
+      <c r="B21" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" s="14"/>
       <c r="D21" s="8"/>
       <c r="E21" s="8"/>
       <c r="F21" s="7">
-        <v>43864</v>
+        <v>43865</v>
       </c>
       <c r="G21" s="7">
-        <v>43868</v>
-      </c>
-      <c r="H21" s="12" t="s">
-        <v>97</v>
-      </c>
+        <v>43865</v>
+      </c>
+      <c r="H21" s="12"/>
       <c r="I21" s="10"/>
       <c r="J21" s="9"/>
       <c r="K21" s="9"/>
@@ -2297,10 +2341,10 @@
       <c r="M21" s="9"/>
       <c r="N21" s="10"/>
       <c r="O21" s="10"/>
-      <c r="P21" s="10"/>
-      <c r="Q21" s="10"/>
-      <c r="R21" s="10"/>
-      <c r="S21" s="10"/>
+      <c r="P21" s="9"/>
+      <c r="Q21" s="9"/>
+      <c r="R21" s="9"/>
+      <c r="S21" s="9"/>
       <c r="T21" s="10"/>
       <c r="U21" s="10"/>
       <c r="V21" s="10"/>
@@ -2323,31 +2367,33 @@
     </row>
     <row r="22" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A22" s="24"/>
-      <c r="B22" s="27" t="s">
-        <v>98</v>
-      </c>
-      <c r="C22" s="8"/>
+      <c r="B22" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="C22" s="14">
+        <v>1</v>
+      </c>
       <c r="D22" s="8"/>
       <c r="E22" s="8"/>
       <c r="F22" s="7">
+        <v>43864</v>
+      </c>
+      <c r="G22" s="7">
         <v>43868</v>
       </c>
-      <c r="G22" s="7">
-        <v>43872</v>
-      </c>
       <c r="H22" s="12" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="I22" s="10"/>
-      <c r="J22" s="10"/>
-      <c r="K22" s="10"/>
-      <c r="L22" s="10"/>
+      <c r="J22" s="9"/>
+      <c r="K22" s="9"/>
+      <c r="L22" s="9"/>
       <c r="M22" s="9"/>
       <c r="N22" s="10"/>
       <c r="O22" s="10"/>
-      <c r="P22" s="9"/>
-      <c r="Q22" s="9"/>
-      <c r="R22" s="9"/>
+      <c r="P22" s="10"/>
+      <c r="Q22" s="10"/>
+      <c r="R22" s="10"/>
       <c r="S22" s="10"/>
       <c r="T22" s="10"/>
       <c r="U22" s="10"/>
@@ -2371,31 +2417,33 @@
     </row>
     <row r="23" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A23" s="24"/>
-      <c r="B23" s="27" t="s">
-        <v>99</v>
-      </c>
-      <c r="C23" s="8"/>
+      <c r="B23" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="C23" s="14">
+        <v>1</v>
+      </c>
       <c r="D23" s="8"/>
       <c r="E23" s="8"/>
       <c r="F23" s="7">
-        <v>43871</v>
+        <v>43868</v>
       </c>
       <c r="G23" s="7">
-        <v>43873</v>
+        <v>43872</v>
       </c>
       <c r="H23" s="12" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="I23" s="10"/>
       <c r="J23" s="10"/>
       <c r="K23" s="10"/>
       <c r="L23" s="10"/>
-      <c r="M23" s="10"/>
+      <c r="M23" s="9"/>
       <c r="N23" s="10"/>
       <c r="O23" s="10"/>
-      <c r="P23" s="10"/>
-      <c r="Q23" s="10"/>
-      <c r="R23" s="10"/>
+      <c r="P23" s="9"/>
+      <c r="Q23" s="9"/>
+      <c r="R23" s="9"/>
       <c r="S23" s="10"/>
       <c r="T23" s="10"/>
       <c r="U23" s="10"/>
@@ -2419,20 +2467,22 @@
     </row>
     <row r="24" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A24" s="24"/>
-      <c r="B24" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="C24" s="8"/>
+      <c r="B24" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="C24" s="14">
+        <v>1</v>
+      </c>
       <c r="D24" s="8"/>
       <c r="E24" s="8"/>
       <c r="F24" s="7">
-        <v>43865</v>
+        <v>43871</v>
       </c>
       <c r="G24" s="7">
         <v>43873</v>
       </c>
       <c r="H24" s="12" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="I24" s="10"/>
       <c r="J24" s="10"/>
@@ -2467,29 +2517,27 @@
     </row>
     <row r="25" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A25" s="24"/>
-      <c r="B25" s="27" t="s">
-        <v>82</v>
-      </c>
-      <c r="C25" s="8"/>
+      <c r="B25" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="C25" s="14"/>
       <c r="D25" s="8"/>
       <c r="E25" s="8"/>
       <c r="F25" s="7">
         <v>43865</v>
       </c>
       <c r="G25" s="7">
-        <v>43871</v>
-      </c>
-      <c r="H25" s="12" t="s">
-        <v>109</v>
-      </c>
+        <v>43873</v>
+      </c>
+      <c r="H25" s="12"/>
       <c r="I25" s="10"/>
-      <c r="J25" s="9"/>
-      <c r="K25" s="9"/>
-      <c r="L25" s="9"/>
-      <c r="M25" s="9"/>
+      <c r="J25" s="10"/>
+      <c r="K25" s="10"/>
+      <c r="L25" s="10"/>
+      <c r="M25" s="10"/>
       <c r="N25" s="10"/>
       <c r="O25" s="10"/>
-      <c r="P25" s="9"/>
+      <c r="P25" s="10"/>
       <c r="Q25" s="10"/>
       <c r="R25" s="10"/>
       <c r="S25" s="10"/>
@@ -2515,29 +2563,31 @@
     </row>
     <row r="26" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A26" s="24"/>
-      <c r="B26" s="28" t="s">
-        <v>111</v>
-      </c>
-      <c r="C26" s="8"/>
+      <c r="B26" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="C26" s="14">
+        <v>1</v>
+      </c>
       <c r="D26" s="8"/>
       <c r="E26" s="8"/>
       <c r="F26" s="7">
         <v>43865</v>
       </c>
       <c r="G26" s="7">
-        <v>43866</v>
+        <v>43871</v>
       </c>
       <c r="H26" s="12" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="I26" s="10"/>
-      <c r="J26" s="10"/>
-      <c r="K26" s="10"/>
+      <c r="J26" s="9"/>
+      <c r="K26" s="9"/>
       <c r="L26" s="9"/>
       <c r="M26" s="9"/>
       <c r="N26" s="10"/>
       <c r="O26" s="10"/>
-      <c r="P26" s="10"/>
+      <c r="P26" s="9"/>
       <c r="Q26" s="10"/>
       <c r="R26" s="10"/>
       <c r="S26" s="10"/>
@@ -2563,20 +2613,22 @@
     </row>
     <row r="27" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A27" s="24"/>
-      <c r="B27" s="28" t="s">
-        <v>110</v>
-      </c>
-      <c r="C27" s="8"/>
+      <c r="B27" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="C27" s="14">
+        <v>1</v>
+      </c>
       <c r="D27" s="8"/>
       <c r="E27" s="8"/>
       <c r="F27" s="7">
-        <v>43866</v>
+        <v>43865</v>
       </c>
       <c r="G27" s="7">
         <v>43866</v>
       </c>
       <c r="H27" s="12" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
       <c r="I27" s="10"/>
       <c r="J27" s="10"/>
@@ -2611,29 +2663,31 @@
     </row>
     <row r="28" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A28" s="24"/>
-      <c r="B28" s="28" t="s">
-        <v>112</v>
-      </c>
-      <c r="C28" s="8"/>
+      <c r="B28" s="23" t="s">
+        <v>110</v>
+      </c>
+      <c r="C28" s="14">
+        <v>1</v>
+      </c>
       <c r="D28" s="8"/>
       <c r="E28" s="8"/>
       <c r="F28" s="7">
-        <v>43865</v>
+        <v>43866</v>
       </c>
       <c r="G28" s="7">
-        <v>43868</v>
+        <v>43866</v>
       </c>
       <c r="H28" s="12" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="I28" s="10"/>
       <c r="J28" s="10"/>
       <c r="K28" s="10"/>
-      <c r="L28" s="10"/>
+      <c r="L28" s="9"/>
       <c r="M28" s="9"/>
       <c r="N28" s="10"/>
       <c r="O28" s="10"/>
-      <c r="P28" s="9"/>
+      <c r="P28" s="10"/>
       <c r="Q28" s="10"/>
       <c r="R28" s="10"/>
       <c r="S28" s="10"/>
@@ -2659,20 +2713,22 @@
     </row>
     <row r="29" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A29" s="24"/>
-      <c r="B29" s="27" t="s">
-        <v>81</v>
-      </c>
-      <c r="C29" s="8"/>
+      <c r="B29" s="23" t="s">
+        <v>112</v>
+      </c>
+      <c r="C29" s="14">
+        <v>1</v>
+      </c>
       <c r="D29" s="8"/>
       <c r="E29" s="8"/>
       <c r="F29" s="7">
-        <v>43867</v>
+        <v>43865</v>
       </c>
       <c r="G29" s="7">
-        <v>43873</v>
+        <v>43868</v>
       </c>
       <c r="H29" s="12" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="I29" s="10"/>
       <c r="J29" s="10"/>
@@ -2707,20 +2763,22 @@
     </row>
     <row r="30" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A30" s="24"/>
-      <c r="B30" s="27" t="s">
-        <v>83</v>
-      </c>
-      <c r="C30" s="8"/>
+      <c r="B30" s="22" t="s">
+        <v>81</v>
+      </c>
+      <c r="C30" s="14">
+        <v>1</v>
+      </c>
       <c r="D30" s="8"/>
       <c r="E30" s="8"/>
       <c r="F30" s="7">
-        <v>43868</v>
+        <v>43867</v>
       </c>
       <c r="G30" s="7">
-        <v>43872</v>
+        <v>43873</v>
       </c>
       <c r="H30" s="12" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="I30" s="10"/>
       <c r="J30" s="10"/>
@@ -2730,7 +2788,7 @@
       <c r="N30" s="10"/>
       <c r="O30" s="10"/>
       <c r="P30" s="9"/>
-      <c r="Q30" s="9"/>
+      <c r="Q30" s="10"/>
       <c r="R30" s="10"/>
       <c r="S30" s="10"/>
       <c r="T30" s="10"/>
@@ -2755,32 +2813,34 @@
     </row>
     <row r="31" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A31" s="24"/>
-      <c r="B31" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="C31" s="8"/>
+      <c r="B31" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="C31" s="14">
+        <v>1</v>
+      </c>
       <c r="D31" s="8"/>
       <c r="E31" s="8"/>
       <c r="F31" s="7">
-        <v>43871</v>
+        <v>43868</v>
       </c>
       <c r="G31" s="7">
         <v>43872</v>
       </c>
       <c r="H31" s="12" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="I31" s="10"/>
       <c r="J31" s="10"/>
       <c r="K31" s="10"/>
       <c r="L31" s="10"/>
-      <c r="M31" s="10"/>
+      <c r="M31" s="9"/>
       <c r="N31" s="10"/>
       <c r="O31" s="10"/>
-      <c r="P31" s="10"/>
+      <c r="P31" s="9"/>
       <c r="Q31" s="9"/>
-      <c r="R31" s="9"/>
-      <c r="S31" s="9"/>
+      <c r="R31" s="10"/>
+      <c r="S31" s="10"/>
       <c r="T31" s="10"/>
       <c r="U31" s="10"/>
       <c r="V31" s="10"/>
@@ -2803,20 +2863,22 @@
     </row>
     <row r="32" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A32" s="24"/>
-      <c r="B32" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="C32" s="8"/>
+      <c r="B32" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="C32" s="14">
+        <v>1</v>
+      </c>
       <c r="D32" s="8"/>
       <c r="E32" s="8"/>
       <c r="F32" s="7">
         <v>43871</v>
       </c>
       <c r="G32" s="7">
-        <v>43874</v>
+        <v>43872</v>
       </c>
       <c r="H32" s="12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I32" s="10"/>
       <c r="J32" s="10"/>
@@ -2825,8 +2887,8 @@
       <c r="M32" s="10"/>
       <c r="N32" s="10"/>
       <c r="O32" s="10"/>
-      <c r="P32" s="9"/>
-      <c r="Q32" s="10"/>
+      <c r="P32" s="10"/>
+      <c r="Q32" s="9"/>
       <c r="R32" s="9"/>
       <c r="S32" s="9"/>
       <c r="T32" s="10"/>
@@ -2851,20 +2913,22 @@
     </row>
     <row r="33" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A33" s="24"/>
-      <c r="B33" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="C33" s="8"/>
+      <c r="B33" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="C33" s="14">
+        <v>1</v>
+      </c>
       <c r="D33" s="8"/>
       <c r="E33" s="8"/>
       <c r="F33" s="7">
         <v>43871</v>
       </c>
       <c r="G33" s="7">
-        <v>43875</v>
+        <v>43874</v>
       </c>
       <c r="H33" s="12" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="I33" s="10"/>
       <c r="J33" s="10"/>
@@ -2876,7 +2940,7 @@
       <c r="P33" s="9"/>
       <c r="Q33" s="10"/>
       <c r="R33" s="9"/>
-      <c r="S33" s="10"/>
+      <c r="S33" s="9"/>
       <c r="T33" s="10"/>
       <c r="U33" s="10"/>
       <c r="V33" s="10"/>
@@ -2899,19 +2963,23 @@
     </row>
     <row r="34" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A34" s="24"/>
-      <c r="B34" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="C34" s="8"/>
+      <c r="B34" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="C34" s="14">
+        <v>1</v>
+      </c>
       <c r="D34" s="8"/>
       <c r="E34" s="8"/>
       <c r="F34" s="7">
         <v>43871</v>
       </c>
       <c r="G34" s="7">
-        <v>43872</v>
-      </c>
-      <c r="H34" s="12"/>
+        <v>43875</v>
+      </c>
+      <c r="H34" s="12" t="s">
+        <v>102</v>
+      </c>
       <c r="I34" s="10"/>
       <c r="J34" s="10"/>
       <c r="K34" s="10"/>
@@ -2919,9 +2987,9 @@
       <c r="M34" s="10"/>
       <c r="N34" s="10"/>
       <c r="O34" s="10"/>
-      <c r="P34" s="10"/>
+      <c r="P34" s="9"/>
       <c r="Q34" s="10"/>
-      <c r="R34" s="10"/>
+      <c r="R34" s="9"/>
       <c r="S34" s="10"/>
       <c r="T34" s="10"/>
       <c r="U34" s="10"/>
@@ -2946,20 +3014,18 @@
     <row r="35" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A35" s="24"/>
       <c r="B35" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="C35" s="8"/>
+        <v>107</v>
+      </c>
+      <c r="C35" s="14"/>
       <c r="D35" s="8"/>
       <c r="E35" s="8"/>
       <c r="F35" s="7">
-        <v>43873</v>
+        <v>43871</v>
       </c>
       <c r="G35" s="7">
-        <v>43874</v>
-      </c>
-      <c r="H35" s="12" t="s">
-        <v>106</v>
-      </c>
+        <v>43872</v>
+      </c>
+      <c r="H35" s="12"/>
       <c r="I35" s="10"/>
       <c r="J35" s="10"/>
       <c r="K35" s="10"/>
@@ -2969,7 +3035,7 @@
       <c r="O35" s="10"/>
       <c r="P35" s="10"/>
       <c r="Q35" s="10"/>
-      <c r="R35" s="9"/>
+      <c r="R35" s="10"/>
       <c r="S35" s="10"/>
       <c r="T35" s="10"/>
       <c r="U35" s="10"/>
@@ -2993,19 +3059,23 @@
     </row>
     <row r="36" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A36" s="24"/>
-      <c r="B36" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C36" s="8"/>
+      <c r="B36" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C36" s="14">
+        <v>1</v>
+      </c>
       <c r="D36" s="8"/>
       <c r="E36" s="8"/>
       <c r="F36" s="7">
         <v>43873</v>
       </c>
       <c r="G36" s="7">
-        <v>43873</v>
-      </c>
-      <c r="H36" s="12"/>
+        <v>43874</v>
+      </c>
+      <c r="H36" s="12" t="s">
+        <v>106</v>
+      </c>
       <c r="I36" s="10"/>
       <c r="J36" s="10"/>
       <c r="K36" s="10"/>
@@ -3015,7 +3085,7 @@
       <c r="O36" s="10"/>
       <c r="P36" s="10"/>
       <c r="Q36" s="10"/>
-      <c r="R36" s="10"/>
+      <c r="R36" s="9"/>
       <c r="S36" s="10"/>
       <c r="T36" s="10"/>
       <c r="U36" s="10"/>
@@ -3039,21 +3109,21 @@
     </row>
     <row r="37" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A37" s="24"/>
-      <c r="B37" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="C37" s="8"/>
+      <c r="B37" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="C37" s="14">
+        <v>1</v>
+      </c>
       <c r="D37" s="8"/>
       <c r="E37" s="8"/>
       <c r="F37" s="7">
         <v>43873</v>
       </c>
       <c r="G37" s="7">
-        <v>43874</v>
-      </c>
-      <c r="H37" s="12" t="s">
-        <v>105</v>
-      </c>
+        <v>43873</v>
+      </c>
+      <c r="H37" s="12"/>
       <c r="I37" s="10"/>
       <c r="J37" s="10"/>
       <c r="K37" s="10"/>
@@ -3087,10 +3157,12 @@
     </row>
     <row r="38" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A38" s="24"/>
-      <c r="B38" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C38" s="8"/>
+      <c r="B38" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="C38" s="14">
+        <v>1</v>
+      </c>
       <c r="D38" s="8"/>
       <c r="E38" s="8"/>
       <c r="F38" s="7">
@@ -3100,7 +3172,7 @@
         <v>43874</v>
       </c>
       <c r="H38" s="12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I38" s="10"/>
       <c r="J38" s="10"/>
@@ -3112,7 +3184,7 @@
       <c r="P38" s="10"/>
       <c r="Q38" s="10"/>
       <c r="R38" s="10"/>
-      <c r="S38" s="9"/>
+      <c r="S38" s="10"/>
       <c r="T38" s="10"/>
       <c r="U38" s="10"/>
       <c r="V38" s="10"/>
@@ -3135,20 +3207,22 @@
     </row>
     <row r="39" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A39" s="24"/>
-      <c r="B39" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="C39" s="8"/>
+      <c r="B39" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="C39" s="14">
+        <v>1</v>
+      </c>
       <c r="D39" s="8"/>
       <c r="E39" s="8"/>
       <c r="F39" s="7">
-        <v>43866</v>
+        <v>43873</v>
       </c>
       <c r="G39" s="7">
         <v>43874</v>
       </c>
       <c r="H39" s="12" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="I39" s="10"/>
       <c r="J39" s="10"/>
@@ -3160,7 +3234,7 @@
       <c r="P39" s="10"/>
       <c r="Q39" s="10"/>
       <c r="R39" s="10"/>
-      <c r="S39" s="10"/>
+      <c r="S39" s="9"/>
       <c r="T39" s="10"/>
       <c r="U39" s="10"/>
       <c r="V39" s="10"/>
@@ -3183,17 +3257,17 @@
     </row>
     <row r="40" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A40" s="24"/>
-      <c r="B40" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="C40" s="8"/>
+      <c r="B40" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="C40" s="14"/>
       <c r="D40" s="8"/>
       <c r="E40" s="8"/>
       <c r="F40" s="7">
-        <v>43867</v>
+        <v>43866</v>
       </c>
       <c r="G40" s="7">
-        <v>43872</v>
+        <v>43874</v>
       </c>
       <c r="H40" s="12" t="s">
         <v>115</v>
@@ -3231,26 +3305,28 @@
     </row>
     <row r="41" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A41" s="24"/>
-      <c r="B41" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="C41" s="8"/>
+      <c r="B41" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="C41" s="14">
+        <v>1</v>
+      </c>
       <c r="D41" s="8"/>
       <c r="E41" s="8"/>
       <c r="F41" s="7">
         <v>43867</v>
       </c>
       <c r="G41" s="7">
-        <v>43870</v>
+        <v>43872</v>
       </c>
       <c r="H41" s="12" t="s">
-        <v>86</v>
+        <v>115</v>
       </c>
       <c r="I41" s="10"/>
       <c r="J41" s="10"/>
       <c r="K41" s="10"/>
-      <c r="L41" s="9"/>
-      <c r="M41" s="9"/>
+      <c r="L41" s="10"/>
+      <c r="M41" s="10"/>
       <c r="N41" s="10"/>
       <c r="O41" s="10"/>
       <c r="P41" s="10"/>
@@ -3279,10 +3355,12 @@
     </row>
     <row r="42" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A42" s="24"/>
-      <c r="B42" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="C42" s="8"/>
+      <c r="B42" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="C42" s="14">
+        <v>1</v>
+      </c>
       <c r="D42" s="8"/>
       <c r="E42" s="8"/>
       <c r="F42" s="7">
@@ -3292,12 +3370,12 @@
         <v>43870</v>
       </c>
       <c r="H42" s="12" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="I42" s="10"/>
       <c r="J42" s="10"/>
       <c r="K42" s="10"/>
-      <c r="L42" s="10"/>
+      <c r="L42" s="9"/>
       <c r="M42" s="9"/>
       <c r="N42" s="10"/>
       <c r="O42" s="10"/>
@@ -3327,17 +3405,19 @@
     </row>
     <row r="43" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A43" s="24"/>
-      <c r="B43" s="18" t="s">
-        <v>116</v>
-      </c>
-      <c r="C43" s="8"/>
+      <c r="B43" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="C43" s="14">
+        <v>1</v>
+      </c>
       <c r="D43" s="8"/>
       <c r="E43" s="8"/>
       <c r="F43" s="7">
-        <v>43868</v>
+        <v>43867</v>
       </c>
       <c r="G43" s="7">
-        <v>43874</v>
+        <v>43870</v>
       </c>
       <c r="H43" s="12" t="s">
         <v>91</v>
@@ -3352,7 +3432,7 @@
       <c r="P43" s="10"/>
       <c r="Q43" s="10"/>
       <c r="R43" s="10"/>
-      <c r="S43" s="9"/>
+      <c r="S43" s="10"/>
       <c r="T43" s="10"/>
       <c r="U43" s="10"/>
       <c r="V43" s="10"/>
@@ -3375,17 +3455,19 @@
     </row>
     <row r="44" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A44" s="24"/>
-      <c r="B44" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="C44" s="8"/>
+      <c r="B44" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="C44" s="14">
+        <v>1</v>
+      </c>
       <c r="D44" s="8"/>
       <c r="E44" s="8"/>
       <c r="F44" s="7">
-        <v>43871</v>
+        <v>43868</v>
       </c>
       <c r="G44" s="7">
-        <v>43873</v>
+        <v>43874</v>
       </c>
       <c r="H44" s="12" t="s">
         <v>91</v>
@@ -3394,13 +3476,13 @@
       <c r="J44" s="10"/>
       <c r="K44" s="10"/>
       <c r="L44" s="10"/>
-      <c r="M44" s="10"/>
+      <c r="M44" s="9"/>
       <c r="N44" s="10"/>
       <c r="O44" s="10"/>
-      <c r="P44" s="9"/>
-      <c r="Q44" s="9"/>
+      <c r="P44" s="10"/>
+      <c r="Q44" s="10"/>
       <c r="R44" s="10"/>
-      <c r="S44" s="10"/>
+      <c r="S44" s="9"/>
       <c r="T44" s="10"/>
       <c r="U44" s="10"/>
       <c r="V44" s="10"/>
@@ -3423,32 +3505,32 @@
     </row>
     <row r="45" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A45" s="24"/>
-      <c r="B45" s="11" t="s">
-        <v>118</v>
-      </c>
-      <c r="C45" s="8"/>
+      <c r="B45" s="21" t="s">
+        <v>117</v>
+      </c>
+      <c r="C45" s="14"/>
       <c r="D45" s="8"/>
       <c r="E45" s="8"/>
       <c r="F45" s="7">
-        <v>43869</v>
+        <v>43871</v>
       </c>
       <c r="G45" s="7">
-        <v>43871</v>
+        <v>43873</v>
       </c>
       <c r="H45" s="12" t="s">
-        <v>119</v>
+        <v>91</v>
       </c>
       <c r="I45" s="10"/>
       <c r="J45" s="10"/>
       <c r="K45" s="10"/>
       <c r="L45" s="10"/>
       <c r="M45" s="10"/>
-      <c r="N45" s="9"/>
-      <c r="O45" s="9"/>
+      <c r="N45" s="10"/>
+      <c r="O45" s="10"/>
       <c r="P45" s="9"/>
       <c r="Q45" s="9"/>
-      <c r="R45" s="9"/>
-      <c r="S45" s="9"/>
+      <c r="R45" s="10"/>
+      <c r="S45" s="10"/>
       <c r="T45" s="10"/>
       <c r="U45" s="10"/>
       <c r="V45" s="10"/>
@@ -3471,19 +3553,23 @@
     </row>
     <row r="46" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A46" s="24"/>
-      <c r="B46" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="C46" s="8"/>
+      <c r="B46" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="C46" s="14">
+        <v>1</v>
+      </c>
       <c r="D46" s="8"/>
       <c r="E46" s="8"/>
       <c r="F46" s="7">
-        <v>43866</v>
+        <v>43881</v>
       </c>
       <c r="G46" s="7">
-        <v>43872</v>
-      </c>
-      <c r="H46" s="12"/>
+        <v>43881</v>
+      </c>
+      <c r="H46" s="12" t="s">
+        <v>124</v>
+      </c>
       <c r="I46" s="10"/>
       <c r="J46" s="10"/>
       <c r="K46" s="10"/>
@@ -3501,7 +3587,7 @@
       <c r="W46" s="10"/>
       <c r="X46" s="10"/>
       <c r="Y46" s="10"/>
-      <c r="Z46" s="10"/>
+      <c r="Z46" s="9"/>
       <c r="AA46" s="10"/>
       <c r="AB46" s="10"/>
       <c r="AC46" s="10"/>
@@ -3517,32 +3603,32 @@
     </row>
     <row r="47" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A47" s="24"/>
-      <c r="B47" s="18" t="s">
-        <v>94</v>
-      </c>
-      <c r="C47" s="8"/>
+      <c r="B47" s="21" t="s">
+        <v>118</v>
+      </c>
+      <c r="C47" s="14"/>
       <c r="D47" s="8"/>
       <c r="E47" s="8"/>
       <c r="F47" s="7">
-        <v>43866</v>
+        <v>43869</v>
       </c>
       <c r="G47" s="7">
-        <v>43867</v>
+        <v>43871</v>
       </c>
       <c r="H47" s="12" t="s">
-        <v>86</v>
+        <v>119</v>
       </c>
       <c r="I47" s="10"/>
       <c r="J47" s="10"/>
       <c r="K47" s="10"/>
       <c r="L47" s="10"/>
       <c r="M47" s="10"/>
-      <c r="N47" s="10"/>
-      <c r="O47" s="10"/>
-      <c r="P47" s="10"/>
+      <c r="N47" s="9"/>
+      <c r="O47" s="9"/>
+      <c r="P47" s="9"/>
       <c r="Q47" s="9"/>
-      <c r="R47" s="10"/>
-      <c r="S47" s="10"/>
+      <c r="R47" s="9"/>
+      <c r="S47" s="9"/>
       <c r="T47" s="10"/>
       <c r="U47" s="10"/>
       <c r="V47" s="10"/>
@@ -3565,21 +3651,19 @@
     </row>
     <row r="48" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A48" s="24"/>
-      <c r="B48" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="C48" s="8"/>
+      <c r="B48" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="C48" s="14"/>
       <c r="D48" s="8"/>
       <c r="E48" s="8"/>
       <c r="F48" s="7">
-        <v>43871</v>
+        <v>43866</v>
       </c>
       <c r="G48" s="7">
         <v>43872</v>
       </c>
-      <c r="H48" s="12" t="s">
-        <v>86</v>
-      </c>
+      <c r="H48" s="12"/>
       <c r="I48" s="10"/>
       <c r="J48" s="10"/>
       <c r="K48" s="10"/>
@@ -3587,8 +3671,8 @@
       <c r="M48" s="10"/>
       <c r="N48" s="10"/>
       <c r="O48" s="10"/>
-      <c r="P48" s="9"/>
-      <c r="Q48" s="9"/>
+      <c r="P48" s="10"/>
+      <c r="Q48" s="10"/>
       <c r="R48" s="10"/>
       <c r="S48" s="10"/>
       <c r="T48" s="10"/>
@@ -3613,17 +3697,17 @@
     </row>
     <row r="49" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A49" s="24"/>
-      <c r="B49" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="C49" s="8"/>
+      <c r="B49" s="22" t="s">
+        <v>94</v>
+      </c>
+      <c r="C49" s="14"/>
       <c r="D49" s="8"/>
       <c r="E49" s="8"/>
       <c r="F49" s="7">
-        <v>43871</v>
+        <v>43866</v>
       </c>
       <c r="G49" s="7">
-        <v>43875</v>
+        <v>43867</v>
       </c>
       <c r="H49" s="12" t="s">
         <v>86</v>
@@ -3635,10 +3719,10 @@
       <c r="M49" s="10"/>
       <c r="N49" s="10"/>
       <c r="O49" s="10"/>
-      <c r="P49" s="9"/>
+      <c r="P49" s="10"/>
       <c r="Q49" s="9"/>
-      <c r="R49" s="9"/>
-      <c r="S49" s="9"/>
+      <c r="R49" s="10"/>
+      <c r="S49" s="10"/>
       <c r="T49" s="10"/>
       <c r="U49" s="10"/>
       <c r="V49" s="10"/>
@@ -3661,20 +3745,20 @@
     </row>
     <row r="50" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A50" s="24"/>
-      <c r="B50" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="C50" s="8"/>
+      <c r="B50" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="C50" s="14"/>
       <c r="D50" s="8"/>
       <c r="E50" s="8"/>
       <c r="F50" s="7">
-        <v>43868</v>
+        <v>43871</v>
       </c>
       <c r="G50" s="7">
-        <v>43875</v>
+        <v>43872</v>
       </c>
       <c r="H50" s="12" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="I50" s="10"/>
       <c r="J50" s="10"/>
@@ -3683,10 +3767,10 @@
       <c r="M50" s="10"/>
       <c r="N50" s="10"/>
       <c r="O50" s="10"/>
-      <c r="P50" s="10"/>
-      <c r="Q50" s="10"/>
-      <c r="R50" s="9"/>
-      <c r="S50" s="9"/>
+      <c r="P50" s="9"/>
+      <c r="Q50" s="9"/>
+      <c r="R50" s="10"/>
+      <c r="S50" s="10"/>
       <c r="T50" s="10"/>
       <c r="U50" s="10"/>
       <c r="V50" s="10"/>
@@ -3709,26 +3793,26 @@
     </row>
     <row r="51" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A51" s="24"/>
-      <c r="B51" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="C51" s="8"/>
+      <c r="B51" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="C51" s="14"/>
       <c r="D51" s="8"/>
       <c r="E51" s="8"/>
       <c r="F51" s="7">
-        <v>43868</v>
+        <v>43871</v>
       </c>
       <c r="G51" s="7">
-        <v>43871</v>
+        <v>43875</v>
       </c>
       <c r="H51" s="12" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="I51" s="10"/>
       <c r="J51" s="10"/>
       <c r="K51" s="10"/>
       <c r="L51" s="10"/>
-      <c r="M51" s="9"/>
+      <c r="M51" s="10"/>
       <c r="N51" s="10"/>
       <c r="O51" s="10"/>
       <c r="P51" s="9"/>
@@ -3757,14 +3841,14 @@
     </row>
     <row r="52" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A52" s="24"/>
-      <c r="B52" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="C52" s="8"/>
+      <c r="B52" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="C52" s="14"/>
       <c r="D52" s="8"/>
       <c r="E52" s="8"/>
       <c r="F52" s="7">
-        <v>43872</v>
+        <v>43868</v>
       </c>
       <c r="G52" s="7">
         <v>43875</v>
@@ -3780,10 +3864,10 @@
       <c r="N52" s="10"/>
       <c r="O52" s="10"/>
       <c r="P52" s="10"/>
-      <c r="Q52" s="9"/>
+      <c r="Q52" s="10"/>
       <c r="R52" s="9"/>
       <c r="S52" s="9"/>
-      <c r="T52" s="9"/>
+      <c r="T52" s="10"/>
       <c r="U52" s="10"/>
       <c r="V52" s="10"/>
       <c r="W52" s="10"/>
@@ -3805,32 +3889,32 @@
     </row>
     <row r="53" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A53" s="24"/>
-      <c r="B53" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="C53" s="8"/>
+      <c r="B53" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="C53" s="14"/>
       <c r="D53" s="8"/>
       <c r="E53" s="8"/>
       <c r="F53" s="7">
+        <v>43868</v>
+      </c>
+      <c r="G53" s="7">
         <v>43871</v>
       </c>
-      <c r="G53" s="7">
-        <v>43872</v>
-      </c>
       <c r="H53" s="12" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="I53" s="10"/>
       <c r="J53" s="10"/>
       <c r="K53" s="10"/>
       <c r="L53" s="10"/>
-      <c r="M53" s="10"/>
+      <c r="M53" s="9"/>
       <c r="N53" s="10"/>
       <c r="O53" s="10"/>
-      <c r="P53" s="10"/>
-      <c r="Q53" s="10"/>
-      <c r="R53" s="10"/>
-      <c r="S53" s="10"/>
+      <c r="P53" s="9"/>
+      <c r="Q53" s="9"/>
+      <c r="R53" s="9"/>
+      <c r="S53" s="9"/>
       <c r="T53" s="10"/>
       <c r="U53" s="10"/>
       <c r="V53" s="10"/>
@@ -3853,33 +3937,33 @@
     </row>
     <row r="54" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A54" s="24"/>
-      <c r="B54" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="C54" s="8"/>
+      <c r="B54" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="C54" s="14"/>
       <c r="D54" s="8"/>
       <c r="E54" s="8"/>
       <c r="F54" s="7">
-        <v>43868</v>
+        <v>43872</v>
       </c>
       <c r="G54" s="7">
-        <v>43872</v>
+        <v>43875</v>
       </c>
       <c r="H54" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="I54" s="10"/>
       <c r="J54" s="10"/>
       <c r="K54" s="10"/>
       <c r="L54" s="10"/>
-      <c r="M54" s="9"/>
+      <c r="M54" s="10"/>
       <c r="N54" s="10"/>
       <c r="O54" s="10"/>
-      <c r="P54" s="9"/>
+      <c r="P54" s="10"/>
       <c r="Q54" s="9"/>
       <c r="R54" s="9"/>
       <c r="S54" s="9"/>
-      <c r="T54" s="10"/>
+      <c r="T54" s="9"/>
       <c r="U54" s="10"/>
       <c r="V54" s="10"/>
       <c r="W54" s="10"/>
@@ -3901,20 +3985,20 @@
     </row>
     <row r="55" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A55" s="24"/>
-      <c r="B55" s="18" t="s">
-        <v>92</v>
-      </c>
-      <c r="C55" s="8"/>
+      <c r="B55" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="C55" s="14"/>
       <c r="D55" s="8"/>
       <c r="E55" s="8"/>
       <c r="F55" s="7">
+        <v>43871</v>
+      </c>
+      <c r="G55" s="7">
         <v>43872</v>
       </c>
-      <c r="G55" s="7">
-        <v>43873</v>
-      </c>
       <c r="H55" s="12" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="I55" s="10"/>
       <c r="J55" s="10"/>
@@ -3925,9 +4009,9 @@
       <c r="O55" s="10"/>
       <c r="P55" s="10"/>
       <c r="Q55" s="10"/>
-      <c r="R55" s="9"/>
-      <c r="S55" s="9"/>
-      <c r="T55" s="9"/>
+      <c r="R55" s="10"/>
+      <c r="S55" s="10"/>
+      <c r="T55" s="10"/>
       <c r="U55" s="10"/>
       <c r="V55" s="10"/>
       <c r="W55" s="10"/>
@@ -3949,32 +4033,32 @@
     </row>
     <row r="56" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A56" s="24"/>
-      <c r="B56" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="C56" s="8"/>
+      <c r="B56" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="C56" s="14"/>
       <c r="D56" s="8"/>
       <c r="E56" s="8"/>
       <c r="F56" s="7">
-        <v>43874</v>
+        <v>43868</v>
       </c>
       <c r="G56" s="7">
-        <v>43875</v>
+        <v>43872</v>
       </c>
       <c r="H56" s="12" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="I56" s="10"/>
       <c r="J56" s="10"/>
       <c r="K56" s="10"/>
       <c r="L56" s="10"/>
-      <c r="M56" s="10"/>
+      <c r="M56" s="9"/>
       <c r="N56" s="10"/>
       <c r="O56" s="10"/>
-      <c r="P56" s="10"/>
-      <c r="Q56" s="10"/>
-      <c r="R56" s="10"/>
-      <c r="S56" s="10"/>
+      <c r="P56" s="9"/>
+      <c r="Q56" s="9"/>
+      <c r="R56" s="9"/>
+      <c r="S56" s="9"/>
       <c r="T56" s="10"/>
       <c r="U56" s="10"/>
       <c r="V56" s="10"/>
@@ -3997,20 +4081,20 @@
     </row>
     <row r="57" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A57" s="24"/>
-      <c r="B57" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="C57" s="8"/>
+      <c r="B57" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="C57" s="14"/>
       <c r="D57" s="8"/>
       <c r="E57" s="8"/>
       <c r="F57" s="7">
-        <v>43874</v>
+        <v>43872</v>
       </c>
       <c r="G57" s="7">
-        <v>43875</v>
+        <v>43873</v>
       </c>
       <c r="H57" s="12" t="s">
-        <v>121</v>
+        <v>91</v>
       </c>
       <c r="I57" s="10"/>
       <c r="J57" s="10"/>
@@ -4021,7 +4105,7 @@
       <c r="O57" s="10"/>
       <c r="P57" s="10"/>
       <c r="Q57" s="10"/>
-      <c r="R57" s="10"/>
+      <c r="R57" s="9"/>
       <c r="S57" s="9"/>
       <c r="T57" s="9"/>
       <c r="U57" s="10"/>
@@ -4045,20 +4129,20 @@
     </row>
     <row r="58" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A58" s="24"/>
-      <c r="B58" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="C58" s="8"/>
+      <c r="B58" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="C58" s="14"/>
       <c r="D58" s="8"/>
       <c r="E58" s="8"/>
       <c r="F58" s="7">
-        <v>43875</v>
+        <v>43874</v>
       </c>
       <c r="G58" s="7">
         <v>43875</v>
       </c>
       <c r="H58" s="12" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="I58" s="10"/>
       <c r="J58" s="10"/>
@@ -4071,7 +4155,7 @@
       <c r="Q58" s="10"/>
       <c r="R58" s="10"/>
       <c r="S58" s="10"/>
-      <c r="T58" s="9"/>
+      <c r="T58" s="10"/>
       <c r="U58" s="10"/>
       <c r="V58" s="10"/>
       <c r="W58" s="10"/>
@@ -4093,20 +4177,20 @@
     </row>
     <row r="59" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A59" s="24"/>
-      <c r="B59" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="C59" s="8"/>
+      <c r="B59" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="C59" s="14"/>
       <c r="D59" s="8"/>
       <c r="E59" s="8"/>
       <c r="F59" s="7">
-        <v>43875</v>
+        <v>43874</v>
       </c>
       <c r="G59" s="7">
         <v>43875</v>
       </c>
       <c r="H59" s="12" t="s">
-        <v>97</v>
+        <v>121</v>
       </c>
       <c r="I59" s="10"/>
       <c r="J59" s="10"/>
@@ -4118,7 +4202,7 @@
       <c r="P59" s="10"/>
       <c r="Q59" s="10"/>
       <c r="R59" s="10"/>
-      <c r="S59" s="10"/>
+      <c r="S59" s="9"/>
       <c r="T59" s="9"/>
       <c r="U59" s="10"/>
       <c r="V59" s="10"/>
@@ -4139,63 +4223,101 @@
       <c r="AK59" s="8"/>
       <c r="AL59" s="8"/>
     </row>
-    <row r="60" spans="1:38" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="1"/>
-      <c r="B60" s="1"/>
-      <c r="F60" s="2"/>
-      <c r="G60" s="2"/>
-      <c r="I60" s="1"/>
-      <c r="J60" s="1"/>
-      <c r="K60" s="1"/>
-      <c r="L60" s="1"/>
-      <c r="M60" s="1"/>
-      <c r="N60" s="1"/>
-      <c r="O60" s="1"/>
-      <c r="P60" s="1"/>
-      <c r="Q60" s="1"/>
-      <c r="R60" s="1"/>
-      <c r="S60" s="1"/>
-      <c r="T60" s="1"/>
-      <c r="U60" s="1"/>
-      <c r="V60" s="1"/>
-      <c r="W60" s="1"/>
-      <c r="X60" s="1"/>
-      <c r="Y60" s="1"/>
-      <c r="Z60" s="1"/>
-      <c r="AA60" s="1"/>
-      <c r="AB60" s="1"/>
-      <c r="AC60" s="1"/>
-      <c r="AD60" s="1"/>
-      <c r="AE60" s="1"/>
-    </row>
-    <row r="61" spans="1:38" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="1"/>
-      <c r="B61" s="1"/>
-      <c r="F61" s="2"/>
-      <c r="G61" s="2"/>
-      <c r="I61" s="1"/>
-      <c r="J61" s="1"/>
-      <c r="K61" s="1"/>
-      <c r="L61" s="1"/>
-      <c r="M61" s="1"/>
-      <c r="N61" s="1"/>
-      <c r="O61" s="1"/>
-      <c r="P61" s="1"/>
-      <c r="Q61" s="1"/>
-      <c r="R61" s="1"/>
-      <c r="S61" s="1"/>
-      <c r="T61" s="1"/>
-      <c r="U61" s="1"/>
-      <c r="V61" s="1"/>
-      <c r="W61" s="1"/>
-      <c r="X61" s="1"/>
-      <c r="Y61" s="1"/>
-      <c r="Z61" s="1"/>
-      <c r="AA61" s="1"/>
-      <c r="AB61" s="1"/>
-      <c r="AC61" s="1"/>
-      <c r="AD61" s="1"/>
-      <c r="AE61" s="1"/>
+    <row r="60" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="A60" s="24"/>
+      <c r="B60" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="C60" s="14"/>
+      <c r="D60" s="8"/>
+      <c r="E60" s="8"/>
+      <c r="F60" s="7">
+        <v>43875</v>
+      </c>
+      <c r="G60" s="7">
+        <v>43875</v>
+      </c>
+      <c r="H60" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="I60" s="10"/>
+      <c r="J60" s="10"/>
+      <c r="K60" s="10"/>
+      <c r="L60" s="10"/>
+      <c r="M60" s="10"/>
+      <c r="N60" s="10"/>
+      <c r="O60" s="10"/>
+      <c r="P60" s="10"/>
+      <c r="Q60" s="10"/>
+      <c r="R60" s="10"/>
+      <c r="S60" s="10"/>
+      <c r="T60" s="9"/>
+      <c r="U60" s="10"/>
+      <c r="V60" s="10"/>
+      <c r="W60" s="10"/>
+      <c r="X60" s="10"/>
+      <c r="Y60" s="10"/>
+      <c r="Z60" s="10"/>
+      <c r="AA60" s="10"/>
+      <c r="AB60" s="10"/>
+      <c r="AC60" s="10"/>
+      <c r="AD60" s="10"/>
+      <c r="AE60" s="10"/>
+      <c r="AF60" s="8"/>
+      <c r="AG60" s="8"/>
+      <c r="AH60" s="8"/>
+      <c r="AI60" s="8"/>
+      <c r="AJ60" s="8"/>
+      <c r="AK60" s="8"/>
+      <c r="AL60" s="8"/>
+    </row>
+    <row r="61" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="A61" s="24"/>
+      <c r="B61" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="C61" s="14"/>
+      <c r="D61" s="8"/>
+      <c r="E61" s="8"/>
+      <c r="F61" s="7">
+        <v>43875</v>
+      </c>
+      <c r="G61" s="7">
+        <v>43875</v>
+      </c>
+      <c r="H61" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="I61" s="10"/>
+      <c r="J61" s="10"/>
+      <c r="K61" s="10"/>
+      <c r="L61" s="10"/>
+      <c r="M61" s="10"/>
+      <c r="N61" s="10"/>
+      <c r="O61" s="10"/>
+      <c r="P61" s="10"/>
+      <c r="Q61" s="10"/>
+      <c r="R61" s="10"/>
+      <c r="S61" s="10"/>
+      <c r="T61" s="9"/>
+      <c r="U61" s="10"/>
+      <c r="V61" s="10"/>
+      <c r="W61" s="10"/>
+      <c r="X61" s="10"/>
+      <c r="Y61" s="10"/>
+      <c r="Z61" s="10"/>
+      <c r="AA61" s="10"/>
+      <c r="AB61" s="10"/>
+      <c r="AC61" s="10"/>
+      <c r="AD61" s="10"/>
+      <c r="AE61" s="10"/>
+      <c r="AF61" s="8"/>
+      <c r="AG61" s="8"/>
+      <c r="AH61" s="8"/>
+      <c r="AI61" s="8"/>
+      <c r="AJ61" s="8"/>
+      <c r="AK61" s="8"/>
+      <c r="AL61" s="8"/>
     </row>
     <row r="62" spans="1:38" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="1"/>
@@ -4342,19 +4464,77 @@
       <c r="AD66" s="1"/>
       <c r="AE66" s="1"/>
     </row>
+    <row r="67" spans="1:31" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="1"/>
+      <c r="B67" s="1"/>
+      <c r="F67" s="2"/>
+      <c r="G67" s="2"/>
+      <c r="I67" s="1"/>
+      <c r="J67" s="1"/>
+      <c r="K67" s="1"/>
+      <c r="L67" s="1"/>
+      <c r="M67" s="1"/>
+      <c r="N67" s="1"/>
+      <c r="O67" s="1"/>
+      <c r="P67" s="1"/>
+      <c r="Q67" s="1"/>
+      <c r="R67" s="1"/>
+      <c r="S67" s="1"/>
+      <c r="T67" s="1"/>
+      <c r="U67" s="1"/>
+      <c r="V67" s="1"/>
+      <c r="W67" s="1"/>
+      <c r="X67" s="1"/>
+      <c r="Y67" s="1"/>
+      <c r="Z67" s="1"/>
+      <c r="AA67" s="1"/>
+      <c r="AB67" s="1"/>
+      <c r="AC67" s="1"/>
+      <c r="AD67" s="1"/>
+      <c r="AE67" s="1"/>
+    </row>
+    <row r="68" spans="1:31" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="1"/>
+      <c r="B68" s="1"/>
+      <c r="F68" s="2"/>
+      <c r="G68" s="2"/>
+      <c r="I68" s="1"/>
+      <c r="J68" s="1"/>
+      <c r="K68" s="1"/>
+      <c r="L68" s="1"/>
+      <c r="M68" s="1"/>
+      <c r="N68" s="1"/>
+      <c r="O68" s="1"/>
+      <c r="P68" s="1"/>
+      <c r="Q68" s="1"/>
+      <c r="R68" s="1"/>
+      <c r="S68" s="1"/>
+      <c r="T68" s="1"/>
+      <c r="U68" s="1"/>
+      <c r="V68" s="1"/>
+      <c r="W68" s="1"/>
+      <c r="X68" s="1"/>
+      <c r="Y68" s="1"/>
+      <c r="Z68" s="1"/>
+      <c r="AA68" s="1"/>
+      <c r="AB68" s="1"/>
+      <c r="AC68" s="1"/>
+      <c r="AD68" s="1"/>
+      <c r="AE68" s="1"/>
+    </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A5:A10"/>
-    <mergeCell ref="A11:A59"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="E3:E4"/>
     <mergeCell ref="A1:AE1"/>
     <mergeCell ref="F3:F4"/>
     <mergeCell ref="G3:G4"/>
     <mergeCell ref="H3:H4"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="B3:B4"/>
+    <mergeCell ref="A5:A10"/>
+    <mergeCell ref="A12:A61"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="E3:E4"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <printOptions horizontalCentered="1"/>

</xml_diff>